<commit_message>
rkau  add, edit, minus otomatis sum di form
</commit_message>
<xml_diff>
--- a/public/files/penjualan.xlsx
+++ b/public/files/penjualan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t xml:space="preserve">REKAPITULASI PENJUALAN </t>
   </si>
@@ -31,73 +31,73 @@
     <t xml:space="preserve">a</t>
   </si>
   <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golongan Tarif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penjualan (MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendapatan (Rp. Ribu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harga Jual (Rp./kWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trw 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trw 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trw 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trw 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">j</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golongan Tarif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penjualan (MWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendapatan (Rp. Ribu)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harga Jual (Rp./kWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trw 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trw 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trw 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trw 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumlah</t>
   </si>
   <si>
     <t xml:space="preserve">f=b+c+d+e</t>
@@ -860,29 +860,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM59"/>
+  <dimension ref="1:59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="3.59183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.34183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="2" width="14.7959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="2" width="17.6020408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="11.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.56632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.45408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="2" width="15.0102040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="2" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
-      <c r="B1" s="0"/>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -894,14 +894,13 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -913,13 +912,12 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -958,40 +956,39 @@
       <c r="N3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="4" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="I4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="12" t="s">
         <v>21</v>
       </c>
@@ -1005,7 +1002,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>21</v>
@@ -1019,19 +1016,18 @@
       <c r="M5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="10"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -1040,277 +1036,255 @@
       <c r="G6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>26</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="J6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="15" t="s">
-        <v>9</v>
+      <c r="K6" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="N6" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21" t="n">
-        <f aca="false">+SUM(E7:H7)</f>
-        <v>0</v>
-      </c>
+      <c r="H7" s="21" t="n">
+        <f aca="false">+SUM(D7:G7)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="22" t="n">
-        <f aca="false">+SUM(J7:M7)</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="23" t="n">
-        <f aca="false">IFERROR(+N7/I7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="24"/>
+      <c r="M7" s="22" t="n">
+        <f aca="false">+SUM(I7:L7)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="23" t="n">
+        <f aca="false">IFERROR(+M7/H7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="18" t="s">
         <v>32</v>
       </c>
+      <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21" t="n">
-        <f aca="false">+SUM(E8:H8)</f>
-        <v>0</v>
-      </c>
+      <c r="H8" s="21" t="n">
+        <f aca="false">+SUM(D8:G8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="21" t="n">
-        <f aca="false">+SUM(J8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="25" t="n">
-        <f aca="false">IFERROR(+N8/I8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="24"/>
+      <c r="M8" s="21" t="n">
+        <f aca="false">+SUM(I8:L8)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="25" t="n">
+        <f aca="false">IFERROR(+M8/H8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
         <v>33</v>
       </c>
+      <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21" t="n">
-        <f aca="false">+SUM(E9:H9)</f>
-        <v>0</v>
-      </c>
+      <c r="H9" s="21" t="n">
+        <f aca="false">+SUM(D9:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21" t="n">
-        <f aca="false">+SUM(J9:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="25" t="n">
-        <f aca="false">IFERROR(+N9/I9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="24"/>
+      <c r="M9" s="21" t="n">
+        <f aca="false">+SUM(I9:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="25" t="n">
+        <f aca="false">IFERROR(+M9/H9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
         <v>34</v>
       </c>
+      <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21" t="n">
-        <f aca="false">+SUM(E10:H10)</f>
-        <v>0</v>
-      </c>
+      <c r="H10" s="21" t="n">
+        <f aca="false">+SUM(D10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="21" t="n">
-        <f aca="false">+SUM(J10:M10)</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="25" t="n">
-        <f aca="false">IFERROR(+N10/I10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="24"/>
+      <c r="M10" s="21" t="n">
+        <f aca="false">+SUM(I10:L10)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="25" t="n">
+        <f aca="false">IFERROR(+M10/H10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21" t="n">
-        <f aca="false">+SUM(E11:H11)</f>
-        <v>0</v>
-      </c>
+      <c r="H11" s="21" t="n">
+        <f aca="false">+SUM(D11:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="21" t="n">
-        <f aca="false">+SUM(J11:M11)</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="25" t="n">
-        <f aca="false">IFERROR(+N11/I11,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="24"/>
+      <c r="M11" s="21" t="n">
+        <f aca="false">+SUM(I11:L11)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="25" t="n">
+        <f aca="false">IFERROR(+M11/H11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
         <v>36</v>
       </c>
+      <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21" t="n">
-        <f aca="false">+SUM(E12:H12)</f>
-        <v>0</v>
-      </c>
+      <c r="H12" s="21" t="n">
+        <f aca="false">+SUM(D12:G12)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="21" t="n">
-        <f aca="false">+SUM(J12:M12)</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="25" t="n">
-        <f aca="false">IFERROR(+N12/I12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="24"/>
+      <c r="M12" s="21" t="n">
+        <f aca="false">+SUM(I12:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="25" t="n">
+        <f aca="false">IFERROR(+M12/H12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21" t="n">
-        <f aca="false">+SUM(E13:H13)</f>
-        <v>0</v>
-      </c>
+      <c r="H13" s="21" t="n">
+        <f aca="false">+SUM(D13:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="21" t="n">
-        <f aca="false">+SUM(J13:M13)</f>
-        <v>0</v>
-      </c>
-      <c r="O13" s="25" t="n">
-        <f aca="false">IFERROR(+N13/I13,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="24"/>
+      <c r="M13" s="21" t="n">
+        <f aca="false">+SUM(I13:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="25" t="n">
+        <f aca="false">IFERROR(+M13/H13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="24"/>
     </row>
     <row r="14" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="27" t="s">
+      <c r="B14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28" t="n">
+        <f aca="false">+SUM(D7:D13)</f>
+        <v>0</v>
+      </c>
       <c r="E14" s="28" t="n">
         <f aca="false">+SUM(E7:E13)</f>
         <v>0</v>
@@ -1347,307 +1321,281 @@
         <f aca="false">+SUM(M7:M13)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="28" t="n">
-        <f aca="false">+SUM(N7:N13)</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="29" t="n">
-        <f aca="false">IFERROR(+N14/I14,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="24"/>
+      <c r="N14" s="29" t="n">
+        <f aca="false">IFERROR(+M14/H14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="24"/>
+      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="C15" s="32" t="s">
         <v>41</v>
       </c>
+      <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34" t="n">
-        <f aca="false">+SUM(E15:H15)</f>
-        <v>0</v>
-      </c>
+      <c r="H15" s="34" t="n">
+        <f aca="false">+SUM(D15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="33"/>
       <c r="J15" s="33"/>
       <c r="K15" s="33"/>
       <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="34" t="n">
-        <f aca="false">+SUM(J15:M15)</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="35" t="n">
-        <f aca="false">IFERROR(+N15/I15,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="24"/>
+      <c r="M15" s="34" t="n">
+        <f aca="false">+SUM(I15:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="35" t="n">
+        <f aca="false">IFERROR(+M15/H15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>41</v>
       </c>
+      <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21" t="n">
-        <f aca="false">+SUM(E16:H16)</f>
-        <v>0</v>
-      </c>
+      <c r="H16" s="21" t="n">
+        <f aca="false">+SUM(D16:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="21" t="n">
-        <f aca="false">+SUM(J16:M16)</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="25" t="n">
-        <f aca="false">IFERROR(+N16/I16,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="24"/>
+      <c r="M16" s="21" t="n">
+        <f aca="false">+SUM(I16:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="25" t="n">
+        <f aca="false">IFERROR(+M16/H16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="C17" s="18" t="s">
         <v>43</v>
       </c>
+      <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21" t="n">
-        <f aca="false">+SUM(E17:H17)</f>
-        <v>0</v>
-      </c>
+      <c r="H17" s="21" t="n">
+        <f aca="false">+SUM(D17:G17)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="21" t="n">
-        <f aca="false">+SUM(J17:M17)</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="25" t="n">
-        <f aca="false">IFERROR(+N17/I17,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="24"/>
+      <c r="M17" s="21" t="n">
+        <f aca="false">+SUM(I17:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="25" t="n">
+        <f aca="false">IFERROR(+M17/H17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>43</v>
       </c>
+      <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="21" t="n">
-        <f aca="false">+SUM(E18:H18)</f>
-        <v>0</v>
-      </c>
+      <c r="H18" s="21" t="n">
+        <f aca="false">+SUM(D18:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="21" t="n">
-        <f aca="false">+SUM(J18:M18)</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="25" t="n">
-        <f aca="false">IFERROR(+N18/I18,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="24"/>
+      <c r="M18" s="21" t="n">
+        <f aca="false">+SUM(I18:L18)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="25" t="n">
+        <f aca="false">IFERROR(+M18/H18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="18" t="s">
         <v>34</v>
       </c>
+      <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21" t="n">
-        <f aca="false">+SUM(E19:H19)</f>
-        <v>0</v>
-      </c>
+      <c r="H19" s="21" t="n">
+        <f aca="false">+SUM(D19:G19)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="20"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="21" t="n">
-        <f aca="false">+SUM(J19:M19)</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="25" t="n">
-        <f aca="false">IFERROR(+N19/I19,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="24"/>
+      <c r="M19" s="21" t="n">
+        <f aca="false">+SUM(I19:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="25" t="n">
+        <f aca="false">IFERROR(+M19/H19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B20" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>44</v>
       </c>
+      <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21" t="n">
-        <f aca="false">+SUM(E20:H20)</f>
-        <v>0</v>
-      </c>
+      <c r="H20" s="21" t="n">
+        <f aca="false">+SUM(D20:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="21" t="n">
-        <f aca="false">+SUM(J20:M20)</f>
-        <v>0</v>
-      </c>
-      <c r="O20" s="25" t="n">
-        <f aca="false">IFERROR(+N20/I20,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="24"/>
+      <c r="M20" s="21" t="n">
+        <f aca="false">+SUM(I20:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="25" t="n">
+        <f aca="false">IFERROR(+M20/H20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="18" t="s">
         <v>46</v>
       </c>
+      <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21" t="n">
-        <f aca="false">+SUM(E21:H21)</f>
-        <v>0</v>
-      </c>
+      <c r="H21" s="21" t="n">
+        <f aca="false">+SUM(D21:G21)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="21" t="n">
-        <f aca="false">+SUM(J21:M21)</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="25" t="n">
-        <f aca="false">IFERROR(+N21/I21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="24"/>
+      <c r="M21" s="21" t="n">
+        <f aca="false">+SUM(I21:L21)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="25" t="n">
+        <f aca="false">IFERROR(+M21/H21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="18" t="s">
         <v>48</v>
       </c>
+      <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21" t="n">
-        <f aca="false">+SUM(E22:H22)</f>
-        <v>0</v>
-      </c>
+      <c r="H22" s="21" t="n">
+        <f aca="false">+SUM(D22:G22)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="21" t="n">
-        <f aca="false">+SUM(J22:M22)</f>
-        <v>0</v>
-      </c>
-      <c r="O22" s="25" t="n">
-        <f aca="false">IFERROR(+N22/I22,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="24"/>
+      <c r="M22" s="21" t="n">
+        <f aca="false">+SUM(I22:L22)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="25" t="n">
+        <f aca="false">IFERROR(+M22/H22,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="24"/>
     </row>
     <row r="23" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="36" t="n">
         <v>17</v>
       </c>
-      <c r="B23" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="C23" s="27" t="s">
+      <c r="B23" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28" t="n">
+        <f aca="false">+SUM(D15:D22)</f>
+        <v>0</v>
+      </c>
       <c r="E23" s="28" t="n">
         <f aca="false">+SUM(E15:E22)</f>
         <v>0</v>
@@ -1684,231 +1632,211 @@
         <f aca="false">+SUM(M15:M22)</f>
         <v>0</v>
       </c>
-      <c r="N23" s="28" t="n">
-        <f aca="false">+SUM(N15:N22)</f>
-        <v>0</v>
-      </c>
-      <c r="O23" s="29" t="n">
-        <f aca="false">IFERROR(+N23/I23,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="24"/>
+      <c r="N23" s="29" t="n">
+        <f aca="false">IFERROR(+M23/H23,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="24"/>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C24" s="31" t="s">
+      <c r="B24" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="C24" s="32" t="s">
         <v>32</v>
       </c>
+      <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34" t="n">
-        <f aca="false">+SUM(E24:H24)</f>
-        <v>0</v>
-      </c>
+      <c r="H24" s="34" t="n">
+        <f aca="false">+SUM(D24:G24)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="33"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="34" t="n">
-        <f aca="false">+SUM(J24:M24)</f>
-        <v>0</v>
-      </c>
-      <c r="O24" s="35" t="n">
-        <f aca="false">IFERROR(+N24/I24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="24"/>
+      <c r="M24" s="34" t="n">
+        <f aca="false">+SUM(I24:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="35" t="n">
+        <f aca="false">IFERROR(+M24/H24,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B25" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="s">
         <v>51</v>
       </c>
+      <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="21" t="n">
-        <f aca="false">+SUM(E25:H25)</f>
-        <v>0</v>
-      </c>
+      <c r="H25" s="21" t="n">
+        <f aca="false">+SUM(D25:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="20"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="21" t="n">
-        <f aca="false">+SUM(J25:M25)</f>
-        <v>0</v>
-      </c>
-      <c r="O25" s="25" t="n">
-        <f aca="false">IFERROR(+N25/I25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="24"/>
+      <c r="M25" s="21" t="n">
+        <f aca="false">+SUM(I25:L25)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="25" t="n">
+        <f aca="false">IFERROR(+M25/H25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="21" t="n">
-        <f aca="false">+SUM(E26:H26)</f>
-        <v>0</v>
-      </c>
+      <c r="H26" s="21" t="n">
+        <f aca="false">+SUM(D26:G26)</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="20"/>
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="21" t="n">
-        <f aca="false">+SUM(J26:M26)</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="25" t="n">
-        <f aca="false">IFERROR(+N26/I26,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="24"/>
+      <c r="M26" s="21" t="n">
+        <f aca="false">+SUM(I26:L26)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="25" t="n">
+        <f aca="false">IFERROR(+M26/H26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B27" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="21" t="n">
-        <f aca="false">+SUM(E27:H27)</f>
-        <v>0</v>
-      </c>
+      <c r="H27" s="21" t="n">
+        <f aca="false">+SUM(D27:G27)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="20"/>
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="21" t="n">
-        <f aca="false">+SUM(J27:M27)</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="25" t="n">
-        <f aca="false">IFERROR(+N27/I27,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="24"/>
+      <c r="M27" s="21" t="n">
+        <f aca="false">+SUM(I27:L27)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="25" t="n">
+        <f aca="false">IFERROR(+M27/H27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="B28" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C28" s="17" t="s">
+      <c r="B28" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="C28" s="18" t="s">
         <v>54</v>
       </c>
+      <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="21" t="n">
-        <f aca="false">+SUM(E28:H28)</f>
-        <v>0</v>
-      </c>
+      <c r="H28" s="21" t="n">
+        <f aca="false">+SUM(D28:G28)</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="20"/>
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="21" t="n">
-        <f aca="false">+SUM(J28:M28)</f>
-        <v>0</v>
-      </c>
-      <c r="O28" s="25" t="n">
-        <f aca="false">IFERROR(+N28/I28,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="24"/>
+      <c r="M28" s="21" t="n">
+        <f aca="false">+SUM(I28:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="25" t="n">
+        <f aca="false">IFERROR(+M28/H28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B29" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C29" s="17" t="s">
+      <c r="B29" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="C29" s="18" t="s">
         <v>56</v>
       </c>
+      <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21" t="n">
-        <f aca="false">+SUM(E29:H29)</f>
-        <v>0</v>
-      </c>
+      <c r="H29" s="21" t="n">
+        <f aca="false">+SUM(D29:G29)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="20"/>
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="21" t="n">
-        <f aca="false">+SUM(J29:M29)</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="25" t="n">
-        <f aca="false">IFERROR(+N29/I29,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="24"/>
+      <c r="M29" s="21" t="n">
+        <f aca="false">+SUM(I29:L29)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="25" t="n">
+        <f aca="false">IFERROR(+M29/H29,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="24"/>
     </row>
     <row r="30" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="36" t="n">
         <v>24</v>
       </c>
-      <c r="B30" s="36" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" s="27" t="s">
+      <c r="B30" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28" t="n">
+        <f aca="false">+SUM(D24:D29)</f>
+        <v>0</v>
+      </c>
       <c r="E30" s="28" t="n">
         <f aca="false">+SUM(E24:E29)</f>
         <v>0</v>
@@ -1945,299 +1873,273 @@
         <f aca="false">+SUM(M24:M29)</f>
         <v>0</v>
       </c>
-      <c r="N30" s="28" t="n">
-        <f aca="false">+SUM(N24:N29)</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="29" t="n">
-        <f aca="false">IFERROR(+N30/I30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="24"/>
+      <c r="N30" s="29" t="n">
+        <f aca="false">IFERROR(+M30/H30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="24"/>
+      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B31" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C31" s="31" t="s">
+      <c r="B31" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="C31" s="32" t="s">
         <v>41</v>
       </c>
+      <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="34" t="n">
-        <f aca="false">+SUM(E31:H31)</f>
-        <v>0</v>
-      </c>
+      <c r="H31" s="34" t="n">
+        <f aca="false">+SUM(D31:G31)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="33"/>
       <c r="J31" s="33"/>
       <c r="K31" s="33"/>
       <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="34" t="n">
-        <f aca="false">+SUM(J31:M31)</f>
-        <v>0</v>
-      </c>
-      <c r="O31" s="35" t="n">
-        <f aca="false">IFERROR(+N31/I31,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="24"/>
+      <c r="M31" s="34" t="n">
+        <f aca="false">+SUM(I31:L31)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="35" t="n">
+        <f aca="false">IFERROR(+M31/H31,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="B32" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18" t="s">
         <v>43</v>
       </c>
+      <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="21" t="n">
-        <f aca="false">+SUM(E32:H32)</f>
-        <v>0</v>
-      </c>
+      <c r="H32" s="21" t="n">
+        <f aca="false">+SUM(D32:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="20"/>
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="21" t="n">
-        <f aca="false">+SUM(J32:M32)</f>
-        <v>0</v>
-      </c>
-      <c r="O32" s="25" t="n">
-        <f aca="false">IFERROR(+N32/I32,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="24"/>
+      <c r="M32" s="21" t="n">
+        <f aca="false">+SUM(I32:L32)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="25" t="n">
+        <f aca="false">IFERROR(+M32/H32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="24"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="B33" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18" t="s">
+      <c r="B33" s="17"/>
+      <c r="C33" s="18" t="s">
         <v>59</v>
       </c>
+      <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="21" t="n">
-        <f aca="false">+SUM(E33:H33)</f>
-        <v>0</v>
-      </c>
+      <c r="H33" s="21" t="n">
+        <f aca="false">+SUM(D33:G33)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="21" t="n">
-        <f aca="false">+SUM(J33:M33)</f>
-        <v>0</v>
-      </c>
-      <c r="O33" s="25" t="n">
-        <f aca="false">IFERROR(+N33/I33,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="24"/>
+      <c r="M33" s="21" t="n">
+        <f aca="false">+SUM(I33:L33)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="25" t="n">
+        <f aca="false">IFERROR(+M33/H33,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="24"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B34" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18" t="s">
         <v>44</v>
       </c>
+      <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="21" t="n">
-        <f aca="false">+SUM(E34:H34)</f>
-        <v>0</v>
-      </c>
+      <c r="H34" s="21" t="n">
+        <f aca="false">+SUM(D34:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="20"/>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="21" t="n">
-        <f aca="false">+SUM(J34:M34)</f>
-        <v>0</v>
-      </c>
-      <c r="O34" s="25" t="n">
-        <f aca="false">IFERROR(+N34/I34,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="24"/>
+      <c r="M34" s="21" t="n">
+        <f aca="false">+SUM(I34:L34)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="25" t="n">
+        <f aca="false">IFERROR(+M34/H34,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B35" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="D35" s="20"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="21" t="n">
-        <f aca="false">+SUM(E35:H35)</f>
-        <v>0</v>
-      </c>
+      <c r="H35" s="21" t="n">
+        <f aca="false">+SUM(D35:G35)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="20"/>
       <c r="J35" s="20"/>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="21" t="n">
-        <f aca="false">+SUM(J35:M35)</f>
-        <v>0</v>
-      </c>
-      <c r="O35" s="25" t="n">
-        <f aca="false">IFERROR(+N35/I35,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="24"/>
+      <c r="M35" s="21" t="n">
+        <f aca="false">+SUM(I35:L35)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="25" t="n">
+        <f aca="false">IFERROR(+M35/H35,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="24"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="B36" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C36" s="17" t="s">
+      <c r="B36" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="C36" s="18" t="s">
         <v>62</v>
       </c>
+      <c r="D36" s="20"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="21" t="n">
-        <f aca="false">+SUM(E36:H36)</f>
-        <v>0</v>
-      </c>
+      <c r="H36" s="21" t="n">
+        <f aca="false">+SUM(D36:G36)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="20"/>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="21" t="n">
-        <f aca="false">+SUM(J36:M36)</f>
-        <v>0</v>
-      </c>
-      <c r="O36" s="25" t="n">
-        <f aca="false">IFERROR(+N36/I36,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q36" s="24"/>
+      <c r="M36" s="21" t="n">
+        <f aca="false">+SUM(I36:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="25" t="n">
+        <f aca="false">IFERROR(+M36/H36,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="24"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="B37" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C37" s="17" t="s">
+      <c r="B37" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="C37" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="D37" s="20"/>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="21" t="n">
-        <f aca="false">+SUM(E37:H37)</f>
-        <v>0</v>
-      </c>
+      <c r="H37" s="21" t="n">
+        <f aca="false">+SUM(D37:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="20"/>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="21" t="n">
-        <f aca="false">+SUM(J37:M37)</f>
-        <v>0</v>
-      </c>
-      <c r="O37" s="25" t="n">
-        <f aca="false">IFERROR(+N37/I37,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q37" s="24"/>
+      <c r="M37" s="21" t="n">
+        <f aca="false">+SUM(I37:L37)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="25" t="n">
+        <f aca="false">IFERROR(+M37/H37,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="24"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="B38" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="C38" s="18" t="s">
         <v>65</v>
       </c>
+      <c r="D38" s="20"/>
       <c r="E38" s="20"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="21" t="n">
-        <f aca="false">+SUM(E38:H38)</f>
-        <v>0</v>
-      </c>
+      <c r="H38" s="21" t="n">
+        <f aca="false">+SUM(D38:G38)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="20"/>
       <c r="J38" s="20"/>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="21" t="n">
-        <f aca="false">+SUM(J38:M38)</f>
-        <v>0</v>
-      </c>
-      <c r="O38" s="25" t="n">
-        <f aca="false">IFERROR(+N38/I38,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q38" s="24"/>
+      <c r="M38" s="21" t="n">
+        <f aca="false">+SUM(I38:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="25" t="n">
+        <f aca="false">IFERROR(+M38/H38,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="24"/>
     </row>
     <row r="39" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="36" t="n">
         <v>33</v>
       </c>
-      <c r="B39" s="36" t="n">
-        <v>4</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="27"/>
+      <c r="B39" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28" t="n">
+        <f aca="false">+SUM(D31:D38)</f>
+        <v>0</v>
+      </c>
       <c r="E39" s="28" t="n">
         <f aca="false">+SUM(E31:E38)</f>
         <v>0</v>
@@ -2274,262 +2176,239 @@
         <f aca="false">+SUM(M31:M38)</f>
         <v>0</v>
       </c>
-      <c r="N39" s="28" t="n">
-        <f aca="false">+SUM(N31:N38)</f>
-        <v>0</v>
-      </c>
-      <c r="O39" s="29" t="n">
-        <f aca="false">IFERROR(+N39/I39,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q39" s="24"/>
+      <c r="N39" s="29" t="n">
+        <f aca="false">IFERROR(+M39/H39,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="24"/>
+      <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="B40" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C40" s="31" t="s">
+      <c r="B40" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="C40" s="32" t="s">
         <v>32</v>
       </c>
+      <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="34" t="n">
-        <f aca="false">+SUM(E40:H40)</f>
-        <v>0</v>
-      </c>
+      <c r="H40" s="34" t="n">
+        <f aca="false">+SUM(D40:G40)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="33"/>
       <c r="J40" s="33"/>
       <c r="K40" s="33"/>
       <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="34" t="n">
-        <f aca="false">+SUM(J40:M40)</f>
-        <v>0</v>
-      </c>
-      <c r="O40" s="35" t="n">
-        <f aca="false">IFERROR(+N40/I40,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="24"/>
+      <c r="M40" s="34" t="n">
+        <f aca="false">+SUM(I40:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="35" t="n">
+        <f aca="false">IFERROR(+M40/H40,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="B41" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="18" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18" t="s">
         <v>51</v>
       </c>
+      <c r="D41" s="20"/>
       <c r="E41" s="20"/>
       <c r="F41" s="20"/>
       <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="21" t="n">
-        <f aca="false">+SUM(E41:H41)</f>
-        <v>0</v>
-      </c>
+      <c r="H41" s="21" t="n">
+        <f aca="false">+SUM(D41:G41)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="20"/>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
       <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="21" t="n">
-        <f aca="false">+SUM(J41:M41)</f>
-        <v>0</v>
-      </c>
-      <c r="O41" s="25" t="n">
-        <f aca="false">IFERROR(+N41/I41,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q41" s="24"/>
+      <c r="M41" s="21" t="n">
+        <f aca="false">+SUM(I41:L41)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="25" t="n">
+        <f aca="false">IFERROR(+M41/H41,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P41" s="24"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="B42" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18" t="s">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
       <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="21" t="n">
-        <f aca="false">+SUM(E42:H42)</f>
-        <v>0</v>
-      </c>
+      <c r="H42" s="21" t="n">
+        <f aca="false">+SUM(D42:G42)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="20"/>
       <c r="J42" s="20"/>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="21" t="n">
-        <f aca="false">+SUM(J42:M42)</f>
-        <v>0</v>
-      </c>
-      <c r="O42" s="25" t="n">
-        <f aca="false">IFERROR(+N42/I42,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q42" s="24"/>
+      <c r="M42" s="21" t="n">
+        <f aca="false">+SUM(I42:L42)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="25" t="n">
+        <f aca="false">IFERROR(+M42/H42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="B43" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="21" t="n">
-        <f aca="false">+SUM(E43:H43)</f>
-        <v>0</v>
-      </c>
+      <c r="H43" s="21" t="n">
+        <f aca="false">+SUM(D43:G43)</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
       <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="21" t="n">
-        <f aca="false">+SUM(J43:M43)</f>
-        <v>0</v>
-      </c>
-      <c r="O43" s="25" t="n">
-        <f aca="false">IFERROR(+N43/I43,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="24"/>
+      <c r="M43" s="21" t="n">
+        <f aca="false">+SUM(I43:L43)</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="25" t="n">
+        <f aca="false">IFERROR(+M43/H43,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="B44" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="18" t="s">
         <v>67</v>
       </c>
+      <c r="D44" s="20"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="21" t="n">
-        <f aca="false">+SUM(E44:H44)</f>
-        <v>0</v>
-      </c>
+      <c r="H44" s="21" t="n">
+        <f aca="false">+SUM(D44:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="21" t="n">
-        <f aca="false">+SUM(J44:M44)</f>
-        <v>0</v>
-      </c>
-      <c r="O44" s="25" t="n">
-        <f aca="false">IFERROR(+N44/I44,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q44" s="24"/>
+      <c r="M44" s="21" t="n">
+        <f aca="false">+SUM(I44:L44)</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="25" t="n">
+        <f aca="false">IFERROR(+M44/H44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P44" s="24"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="B45" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C45" s="17" t="s">
+      <c r="B45" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="C45" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="D45" s="20"/>
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="21" t="n">
-        <f aca="false">+SUM(E45:H45)</f>
-        <v>0</v>
-      </c>
+      <c r="H45" s="21" t="n">
+        <f aca="false">+SUM(D45:G45)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
       <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="21" t="n">
-        <f aca="false">+SUM(J45:M45)</f>
-        <v>0</v>
-      </c>
-      <c r="O45" s="25" t="n">
-        <f aca="false">IFERROR(+N45/I45,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q45" s="24"/>
+      <c r="M45" s="21" t="n">
+        <f aca="false">+SUM(I45:L45)</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="25" t="n">
+        <f aca="false">IFERROR(+M45/H45,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P45" s="24"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="B46" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C46" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
       <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="21" t="n">
-        <f aca="false">+SUM(E46:H46)</f>
-        <v>0</v>
-      </c>
+      <c r="H46" s="21" t="n">
+        <f aca="false">+SUM(D46:G46)</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="20"/>
       <c r="J46" s="20"/>
       <c r="K46" s="20"/>
       <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="21" t="n">
-        <f aca="false">+SUM(J46:M46)</f>
-        <v>0</v>
-      </c>
-      <c r="O46" s="25" t="n">
-        <f aca="false">IFERROR(+N46/I46,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q46" s="24"/>
+      <c r="M46" s="21" t="n">
+        <f aca="false">+SUM(I46:L46)</f>
+        <v>0</v>
+      </c>
+      <c r="N46" s="25" t="n">
+        <f aca="false">IFERROR(+M46/H46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P46" s="24"/>
     </row>
     <row r="47" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="36" t="n">
         <v>41</v>
       </c>
-      <c r="B47" s="36" t="n">
-        <v>5</v>
-      </c>
-      <c r="C47" s="27" t="s">
+      <c r="B47" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28" t="n">
+        <f aca="false">+SUM(D40:D46)</f>
+        <v>0</v>
+      </c>
       <c r="E47" s="28" t="n">
         <f aca="false">+SUM(E40:E46)</f>
         <v>0</v>
@@ -2566,132 +2445,121 @@
         <f aca="false">+SUM(M40:M46)</f>
         <v>0</v>
       </c>
-      <c r="N47" s="28" t="n">
-        <f aca="false">+SUM(N40:N46)</f>
-        <v>0</v>
-      </c>
-      <c r="O47" s="29" t="n">
-        <f aca="false">IFERROR(+N47/I47,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="24"/>
+      <c r="N47" s="29" t="n">
+        <f aca="false">IFERROR(+M47/H47,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P47" s="24"/>
+      <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="B48" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C48" s="31" t="s">
+      <c r="B48" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="32" t="s">
+      <c r="C48" s="32" t="s">
         <v>38</v>
       </c>
+      <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="34" t="n">
-        <f aca="false">+SUM(E48:H48)</f>
-        <v>0</v>
-      </c>
+      <c r="H48" s="34" t="n">
+        <f aca="false">+SUM(D48:G48)</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="33"/>
       <c r="J48" s="33"/>
       <c r="K48" s="33"/>
       <c r="L48" s="33"/>
-      <c r="M48" s="33"/>
-      <c r="N48" s="34" t="n">
-        <f aca="false">+SUM(J48:M48)</f>
-        <v>0</v>
-      </c>
-      <c r="O48" s="35" t="n">
-        <f aca="false">IFERROR(+N48/I48,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q48" s="24"/>
+      <c r="M48" s="34" t="n">
+        <f aca="false">+SUM(I48:L48)</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="35" t="n">
+        <f aca="false">IFERROR(+M48/H48,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P48" s="24"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="B49" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C49" s="31" t="s">
+      <c r="B49" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="32" t="s">
+      <c r="C49" s="32" t="s">
         <v>38</v>
       </c>
+      <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="33"/>
       <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="34" t="n">
-        <f aca="false">+SUM(E49:H49)</f>
-        <v>0</v>
-      </c>
+      <c r="H49" s="34" t="n">
+        <f aca="false">+SUM(D49:G49)</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="33"/>
       <c r="J49" s="33"/>
       <c r="K49" s="33"/>
       <c r="L49" s="33"/>
-      <c r="M49" s="33"/>
-      <c r="N49" s="34" t="n">
-        <f aca="false">+SUM(J49:M49)</f>
-        <v>0</v>
-      </c>
-      <c r="O49" s="35" t="n">
-        <f aca="false">IFERROR(+N49/I49,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q49" s="24"/>
+      <c r="M49" s="34" t="n">
+        <f aca="false">+SUM(I49:L49)</f>
+        <v>0</v>
+      </c>
+      <c r="N49" s="35" t="n">
+        <f aca="false">IFERROR(+M49/H49,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P49" s="24"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="n">
         <v>44</v>
       </c>
-      <c r="B50" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C50" s="31" t="s">
+      <c r="B50" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="32" t="s">
+      <c r="C50" s="32" t="s">
         <v>74</v>
       </c>
+      <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="34" t="n">
-        <f aca="false">+SUM(E50:H50)</f>
-        <v>0</v>
-      </c>
+      <c r="H50" s="34" t="n">
+        <f aca="false">+SUM(D50:G50)</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="33"/>
       <c r="J50" s="33"/>
       <c r="K50" s="33"/>
       <c r="L50" s="33"/>
-      <c r="M50" s="33"/>
-      <c r="N50" s="34" t="n">
-        <f aca="false">+SUM(J50:M50)</f>
-        <v>0</v>
-      </c>
-      <c r="O50" s="35" t="n">
-        <f aca="false">IFERROR(+N50/I50,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q50" s="24"/>
+      <c r="M50" s="34" t="n">
+        <f aca="false">+SUM(I50:L50)</f>
+        <v>0</v>
+      </c>
+      <c r="N50" s="35" t="n">
+        <f aca="false">IFERROR(+M50/H50,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P50" s="24"/>
     </row>
     <row r="51" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="36" t="n">
         <v>45</v>
       </c>
-      <c r="B51" s="36" t="n">
-        <v>6</v>
-      </c>
-      <c r="C51" s="37" t="s">
+      <c r="B51" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="38" t="n">
+        <f aca="false">+D50+D49+D48+D47+D39+D30+D23+D14</f>
+        <v>0</v>
+      </c>
       <c r="E51" s="38" t="n">
         <f aca="false">+E50+E49+E48+E47+E39+E30+E23+E14</f>
         <v>0</v>
@@ -2728,23 +2596,18 @@
         <f aca="false">+M50+M49+M48+M47+M39+M30+M23+M14</f>
         <v>0</v>
       </c>
-      <c r="N51" s="38" t="n">
-        <f aca="false">+N50+N49+N48+N47+N39+N30+N23+N14</f>
-        <v>0</v>
-      </c>
-      <c r="O51" s="39" t="n">
-        <f aca="false">IFERROR(+N51/I51,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="24"/>
+      <c r="N51" s="39" t="n">
+        <f aca="false">IFERROR(+M51/H51,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P51" s="24"/>
+      <c r="AMJ51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="n">
         <v>46</v>
       </c>
-      <c r="B52" s="4" t="n">
-        <v>7</v>
-      </c>
+      <c r="D52" s="0"/>
       <c r="E52" s="0"/>
       <c r="F52" s="0"/>
       <c r="G52" s="0"/>
@@ -2755,19 +2618,19 @@
       <c r="L52" s="0"/>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
-      <c r="O52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="n">
         <v>47</v>
       </c>
-      <c r="B53" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="C53" s="40" t="s">
+      <c r="B53" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="41" t="n">
+        <f aca="false">D51-D54</f>
+        <v>0</v>
+      </c>
       <c r="E53" s="41" t="n">
         <f aca="false">E51-E54</f>
         <v>0</v>
@@ -2804,12 +2667,8 @@
         <f aca="false">M51-M54</f>
         <v>0</v>
       </c>
-      <c r="N53" s="41" t="n">
-        <f aca="false">N51-N54</f>
-        <v>0</v>
-      </c>
-      <c r="O53" s="42" t="n">
-        <f aca="false">IFERROR(+N53/I53,0)</f>
+      <c r="N53" s="42" t="n">
+        <f aca="false">IFERROR(+M53/H53,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2817,13 +2676,14 @@
       <c r="A54" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="B54" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="C54" s="43" t="s">
+      <c r="B54" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="44" t="n">
+        <f aca="false">SUM(D16,D18:D22,D28:D29,D37:D38,D44:D46,D50)</f>
+        <v>0</v>
+      </c>
       <c r="E54" s="44" t="n">
         <f aca="false">SUM(E16,E18:E22,E28:E29,E37:E38,E44:E46,E50)</f>
         <v>0</v>
@@ -2860,16 +2720,13 @@
         <f aca="false">SUM(M16,M18:M22,M28:M29,M37:M38,M44:M46,M50)</f>
         <v>0</v>
       </c>
-      <c r="N54" s="44" t="n">
-        <f aca="false">SUM(N16,N18:N22,N28:N29,N37:N38,N44:N46,N50)</f>
-        <v>0</v>
-      </c>
-      <c r="O54" s="45" t="n">
-        <f aca="false">IFERROR(+N54/I54,0)</f>
+      <c r="N54" s="45" t="n">
+        <f aca="false">IFERROR(+M54/H54,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
       <c r="G55" s="0"/>
@@ -2880,12 +2737,12 @@
       <c r="L55" s="0"/>
       <c r="M55" s="0"/>
       <c r="N55" s="0"/>
-      <c r="O55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="46" t="s">
+      <c r="B56" s="46" t="s">
         <v>78</v>
       </c>
+      <c r="C56" s="46"/>
       <c r="D56" s="46"/>
       <c r="E56" s="46"/>
       <c r="F56" s="46"/>
@@ -2898,7 +2755,7 @@
       <c r="M56" s="46"/>
       <c r="N56" s="46"/>
       <c r="O56" s="46"/>
-      <c r="P56" s="46"/>
+      <c r="P56" s="47"/>
       <c r="Q56" s="47"/>
       <c r="R56" s="47"/>
       <c r="S56" s="47"/>
@@ -2921,12 +2778,12 @@
       <c r="AJ56" s="47"/>
       <c r="AK56" s="47"/>
       <c r="AL56" s="47"/>
-      <c r="AM56" s="47"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="48" t="s">
+      <c r="B57" s="48" t="s">
         <v>79</v>
       </c>
+      <c r="C57" s="48"/>
       <c r="D57" s="48"/>
       <c r="E57" s="48"/>
       <c r="F57" s="48"/>
@@ -2962,12 +2819,12 @@
       <c r="AJ57" s="48"/>
       <c r="AK57" s="48"/>
       <c r="AL57" s="48"/>
-      <c r="AM57" s="48"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="48" t="s">
+      <c r="B58" s="48" t="s">
         <v>80</v>
       </c>
+      <c r="C58" s="48"/>
       <c r="D58" s="48"/>
       <c r="E58" s="48"/>
       <c r="F58" s="48"/>
@@ -3003,33 +2860,32 @@
       <c r="AJ58" s="48"/>
       <c r="AK58" s="48"/>
       <c r="AL58" s="48"/>
-      <c r="AM58" s="48"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="0" t="s">
+      <c r="B59" s="0" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="C2:O2"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C56:P56"/>
-    <mergeCell ref="C57:AM57"/>
-    <mergeCell ref="C58:AM58"/>
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B56:O56"/>
+    <mergeCell ref="B57:AL57"/>
+    <mergeCell ref="B58:AL58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>